<commit_message>
Updated JLCPCBA for Toolhead
</commit_message>
<xml_diff>
--- a/PD-Toolhead/V1.2_JLC_PCBA_CPL.xlsx
+++ b/PD-Toolhead/V1.2_JLC_PCBA_CPL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_DATEN\Alexander\Projekte\_Projektordner\3D-Drucker\USB-PD-Hotend\Github_Upload\StealthburnerFullUSBPD\PD-Toolhead\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155CDE76-22AE-4158-9FA6-A7E161ACCC7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A982F8-6845-4D3C-9362-4E9DA1A5AC11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{A81E44D0-CF51-4418-9E54-AE629FEA33B8}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="373">
   <si>
     <t>Designator</t>
   </si>
@@ -1524,8 +1524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4BB55D8-6A12-4119-8779-4CCBC4469CA5}">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2800,6 +2800,9 @@
       <c r="H47" s="1" t="s">
         <v>173</v>
       </c>
+      <c r="I47" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">

</xml_diff>